<commit_message>
update data and TC
</commit_message>
<xml_diff>
--- a/src/test/data/login01.xlsx
+++ b/src/test/data/login01.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>baminh</t>
+  </si>
+  <si>
+    <t>thaovy</t>
   </si>
 </sst>
 </file>
@@ -364,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,6 +391,14 @@
         <v>123</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update to run parallel
</commit_message>
<xml_diff>
--- a/src/test/data/login01.xlsx
+++ b/src/test/data/login01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Username</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>baminh</t>
-  </si>
-  <si>
-    <t>thaovy</t>
   </si>
 </sst>
 </file>
@@ -367,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,14 +388,6 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>123</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>